<commit_message>
updated excel ironpython ansys
</commit_message>
<xml_diff>
--- a/003 Excel from IronPython/ansys.xlsx
+++ b/003 Excel from IronPython/ansys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AnsysScripting\003 Excel from IronPython\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068630A9-BEAE-4432-B482-D73570D2B72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA24F1F-78CA-4D74-BF71-5BE1D5279B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25452" yWindow="3324" windowWidth="17280" windowHeight="8964" xr2:uid="{13942E29-287E-4572-8CCF-8EAF85D5C626}"/>
+    <workbookView xWindow="24672" yWindow="2328" windowWidth="17280" windowHeight="8964" xr2:uid="{13942E29-287E-4572-8CCF-8EAF85D5C626}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -43,16 +43,56 @@
   </si>
   <si>
     <t>dd</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>id1</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>eee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -74,12 +114,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,17 +190,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE33DD84-28E5-4DD5-B4B6-21313CD36A55}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{FE33DD84-28E5-4DD5-B4B6-21313CD36A55}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8945F11E-8A60-4DFA-888E-29100A75DE97}" name="id"/>
-    <tableColumn id="2" xr3:uid="{3FC3183C-A193-471E-A397-465D5EAF1C0E}" name="name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,59 +488,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE1B5DC-8141-4E17-91CC-77153F0B74CB}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
+      <c r="A2" s="3">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3">
+        <v>11</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="3">
+      <c r="A3" s="3">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
+      <c r="A4" s="3">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
+      <c r="A5" s="3">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row spans="1:9" x14ac:dyDescent="0.3" outlineLevel="0" r="6">
+      <c r="A6" s="5">
+        <v>66</v>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>ee</t>
+        </is>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>55</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>